<commit_message>
draft historical and updated social support
</commit_message>
<xml_diff>
--- a/Data/Historical.xlsx
+++ b/Data/Historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B40255D-A1E4-DC4B-952B-EA77BC2F404D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85486E3E-7656-4243-A904-14E970858AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16200" xr2:uid="{663F1AFD-6E9B-E447-A23D-DE2FC8DC025F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t xml:space="preserve">What is your ethnicity? </t>
   </si>
@@ -44,6 +44,75 @@
   </si>
   <si>
     <t>Question:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior to coronavirus (COVID-19), did you get free or reduced lunches for your child(ren)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Yes, my child(ren) received free or reduced lunches  
+• No, my child did not receive free or reduced lunches, but they were available 
+• No, free or reduced lunches were not available for my children  
+• No, but I had planned on getting free or reduced lunches for my children soon  
+• No, I didn't know how to access this resource 
+• Not applicable </t>
+  </si>
+  <si>
+    <t>Meet Basic Needs for Health and Well-Being</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you currently get free or reduced lunches for your child(ren)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Yes, my child(ren) receive(s) free or reduced lunches  
+• No, my child does not receive free or reduced lunches, but they were available 
+• No, free or reduced lunches are not available for my children  
+• No, but I plan on getting free or reduced lunches for my children soon  
+• No, I don't know how to access this resource 
+• Not applicable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the past month, how hard has it been for you to pay for the very basics like food, housing, medical care, and heating? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Very hard 
+• Hard 
+• Somewhat hard  
+• Not very hard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of these needs have been hard to pay for in the past month? Select all that apply.  </t>
+  </si>
+  <si>
+    <t>• Food 
+• Housing 
+• Utilities (electric, water, trash) 
+• Healthcare 
+• Social 
+• Emotional 
+• Childcare 
+• Other (please specify) [text entry] 
+• None of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the biggest challenges and concerns for you and your family right now? </t>
+  </si>
+  <si>
+    <t>Open answer</t>
+  </si>
+  <si>
+    <t>Open Ended Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is helping you and your family the most right now? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is on your mind the most when you think about your community re-opening? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What concerns do you have about your place of employment and/or your child’s child care setting re-opening? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there anything else you would like to tell us about you and your family’s experiences during the COVID-19 pandemic? </t>
   </si>
 </sst>
 </file>
@@ -401,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AAEF64-5CC6-0C4E-8EBE-181A98472300}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -432,6 +501,135 @@
       </c>
       <c r="C2" s="2"/>
     </row>
+    <row r="3" spans="1:4" ht="409.6">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="409.6">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="204">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="306">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="136">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="102">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="153">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="187">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="204">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated historical questions through week 1.
</commit_message>
<xml_diff>
--- a/Data/Historical.xlsx
+++ b/Data/Historical.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1614B9D8-7BCF-224D-83F8-EBC94A60064F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D263594-1F72-CB47-BC45-D9841AEEB88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="16200" xr2:uid="{663F1AFD-6E9B-E447-A23D-DE2FC8DC025F}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="13840" windowHeight="16200" xr2:uid="{663F1AFD-6E9B-E447-A23D-DE2FC8DC025F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$316</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="390">
   <si>
     <t>Source:</t>
   </si>
@@ -1834,6 +1837,238 @@
   </si>
   <si>
     <t>Social Support Special Topic</t>
+  </si>
+  <si>
+    <t>Have you accessed any of the following services/content in an online/digital format during the COVID-19 pandemic? Select all that apply</t>
+  </si>
+  <si>
+    <t>• Medical care for yourself
+• Medical care for your child
+• Mental health care
+• Parenting support
+• Fitness classes
+• Educational courses
+• Other, please describe [Free text]
+• None of the above</t>
+  </si>
+  <si>
+    <t>[If yes to accessed digital content during pandemic]
+Please rate how helpful each of the services you have accessed online/digitally have been on a scale of 0-5.
+0 indicates that you have not accessed this service online/digitally
+For those services you have accessed online/digitally:
+1 indicates accessing this service digitally was not helpful at all and 5 indicates that receiving a service digitally was very helpful</t>
+  </si>
+  <si>
+    <t>• Medical care for yourself [0-5 Scale]
+• Medical care for your child [0-5 Scale]
+• Mental health care [0-5 Scale]
+• Parenting support [0-5 Scale]
+• Fitness classes [0-5 Scale]
+• Educational courses [0-5 Scale]
+• Other, please describe [Free text] [0-5 Scale]
+• None of the above [0-5 Scale]</t>
+  </si>
+  <si>
+    <t>• Cared for by other parent/step parent
+• Cared for by sibling 15 years or older
+• Cared for by grandparent
+• Cared for by other relative
+• Cared for by family day care provider
+• Cared for by other non-relative
+• Cared for by child care center
+• Cared for by a day care that is a Head Start program
+• Cared for in a nursery/preschool
+• Cared for by before/after school program
+• Child(ren) cared for themselves
+• Other, please describe [Free text]</t>
+  </si>
+  <si>
+    <t>Single select from 1-100 and more than than 100</t>
+  </si>
+  <si>
+    <t>Prior to the coronavirus (COVID-19) Pandemic, did you utilize any of the following for childcare? [Also asked currently]</t>
+  </si>
+  <si>
+    <t>Prior to the coronavirus (COVID-19) Pandemic, how many hours on average per week, was your child cared for by [asked for all care options selected]? [Also asked currently]</t>
+  </si>
+  <si>
+    <t>Were you attending school prior to the coronavirus (COVID-19) pandemic?</t>
+  </si>
+  <si>
+    <t>• Yes, Full time
+• Yes, Part time
+• No</t>
+  </si>
+  <si>
+    <t>Since the coronavirus (COVID-19) pandemic, what has changed regarding your education/schooling?</t>
+  </si>
+  <si>
+    <t>[Mulitple Select]
+• Unable to attend classes in person
+• Courses/Schooling offered online/remotely only, and I'm able to participate
+• Courses/Schooling offered online/remotely, but unable to participate
+• Courses/Schooling offered via alternative means (ex. mail, television etc.)
+• Nothing has changed
+• Not continuing in coursework due to pandemic
+• Planned to not continue in coursework, regardless of pandemic</t>
+  </si>
+  <si>
+    <t>Was your child(ren) attending school prior to the coronavirus (COVID-19) pandemic? Select all that apply</t>
+  </si>
+  <si>
+    <t>[Mulitple Select]
+• Unable to attend classes in person
+• Courses/Schooling offered online/remotely only, and ny child is able to participate
+• Courses/Schooling offered online/remotely, but unable to participate
+• Courses/Schooling offered via alternative means (ex. mail, television etc.)
+• Nothing has changed
+• Not continuing in coursework due to pandemic
+• Planned to not continue in coursework, regardless of pandemic</t>
+  </si>
+  <si>
+    <t>Since the coronavirus (COVID-19) pandemic, what has changed for your child(ren) regarding their education/schooling?</t>
+  </si>
+  <si>
+    <t>[If child age 0-5 covered by health insurance]
+What type of health insurance or health care coverage does your child have?</t>
+  </si>
+  <si>
+    <t>•  Private Health Insurance
+•  Medicare
+•  Medicaid
+•  Children's Health Insurance Program (CHIP)
+•  Military related health care (e.g. TRICARE (CHAMPUS) / VA Health Care / CHAMP-VA)
+•  Indian Health Service
+•  State-sponsored health plan
+•  Other government program
+•  I don't know
+• Other, please describe
+• Not applicable</t>
+  </si>
+  <si>
+    <t>[If yes to suspected or diagnosed with COVID]
+To the best of your knowledge, why did you not have a test for coronavirus (COVID-19)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Test not available (ex. Not enough supplies)
+• Didn't meet testing criteria (ex. Some states only test those with symptoms, and who are hospitalized)
+• Physician or Public Health Official did not recommend a test
+• Other [Free Text]
+</t>
+  </si>
+  <si>
+    <t>Have you been hospitalized in 2020?</t>
+  </si>
+  <si>
+    <t>• Yes, for coronavirus (COVID-19)
+• Yes, for something else
+• No</t>
+  </si>
+  <si>
+    <t>Who is the primary breadwinner in your household currently?
+Breadwinner indicates the person in your household with the highest income.</t>
+  </si>
+  <si>
+    <t>• Myself
+• My partner or spouse
+• Relatively equal with my partner or spouse
+• Someone else in my household
+• Not Applicable</t>
+  </si>
+  <si>
+    <t>Has the primary breadwinner changed since the coronavirus (COVID-19) pandemic?
+Example, one person earned more income prior to the pandemic, but now their partner earns more.</t>
+  </si>
+  <si>
+    <t>Which of the following best describes your current employment status? Select all that apply</t>
+  </si>
+  <si>
+    <t>[Multiple Select]
+• Working full time
+• Working part time
+• Unemployed or laid off and seeking employment
+• Unemployed or laid off, not seeking employment
+• Temporarily furloughed
+• Hours reduced
+• Keeping house or raising children full time
+• Retired
+• Full-time student
+• Other [Free Text]</t>
+  </si>
+  <si>
+    <t>Which of the following best describes your employment status prior to the coronavirus (COVID-19) Pandemic? Select all that apply</t>
+  </si>
+  <si>
+    <t>During the coronavirus (COVID-19) pandemic, are you considered an essential employee?</t>
+  </si>
+  <si>
+    <t>[If yes to employer offers sick leave]
+• If yes, has your place of employment increased the amount of paid sick leave provided to you during the coronavirus (COVID-19) Pandemic?</t>
+  </si>
+  <si>
+    <t>[If yes to receiving benefits]
+What types of benefits are you receiving?</t>
+  </si>
+  <si>
+    <t>[Multiple Select]
+• Health / Medical
+• Food
+• Income (not including federal stimulus checks)
+• Disability (not military)
+• Military Pension
+• Military Disability
+• Military Medical Care
+• Housing Subsidy
+• Child Care Subsidy
+• Other, please describe [Free Text]</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified from U.S. Census</t>
+  </si>
+  <si>
+    <t>• No problems
+• Minor problems
+• Major problems
+• Extreme problems</t>
+  </si>
+  <si>
+    <t>What best describes your relationship status?</t>
+  </si>
+  <si>
+    <t>• Engaged
+• Married
+• Separated
+• Divorced
+• Widowed
+• Living together/cohabitating
+• Romantically involved, but living apart
+• Not in any kind of relatinoship (Single)
+• Other</t>
+  </si>
+  <si>
+    <t>• Male
+• Female
+• Transgender Female
+• Transgender Male
+• Gender variant/Non-Conforming
+• Prefer not to answer
+• Other [Free Text]</t>
+  </si>
+  <si>
+    <t>What is your ethnicity?</t>
+  </si>
+  <si>
+    <t>• Hispanic/Latinx
+• Not Hisoanic/Latinx</t>
+  </si>
+  <si>
+    <t>[If pregnant] Approximately how many weeks along are you?</t>
+  </si>
+  <si>
+    <t>Numeric selection 0-50</t>
+  </si>
+  <si>
+    <t>U.S Census</t>
   </si>
 </sst>
 </file>
@@ -1907,7 +2142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1928,6 +2163,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2244,10 +2482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AAEF64-5CC6-0C4E-8EBE-181A98472300}">
-  <dimension ref="A1:D314"/>
+  <dimension ref="A1:D327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3239,7 +3477,7 @@
         <v>152</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>381</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>150</v>
@@ -3952,74 +4190,74 @@
         <v>87</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="102">
+    <row r="128" spans="1:4" ht="119">
       <c r="A128" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="102">
       <c r="A129" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>87</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="119">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="34">
       <c r="A130" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="B130" s="1"/>
       <c r="C130" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="85">
       <c r="A131" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="34">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="85">
       <c r="A132" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B132" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="C132" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="D132" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="133" spans="1:4" ht="85">
       <c r="A133" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>100</v>
@@ -4028,71 +4266,71 @@
         <v>101</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="85">
       <c r="A134" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="85">
       <c r="A135" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="85">
-      <c r="A136" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="85">
-      <c r="A137" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D137" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="306">
-      <c r="A138" s="4" t="s">
+    <row r="136" spans="1:4" ht="306">
+      <c r="A136" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>212</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="306">
+      <c r="A137" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="34">
+      <c r="A138" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>213</v>
@@ -4101,12 +4339,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="306">
-      <c r="A139" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>212</v>
+    <row r="139" spans="1:4" ht="68">
+      <c r="A139" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>213</v>
@@ -4116,11 +4354,11 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="34">
-      <c r="A140" s="1" t="s">
-        <v>215</v>
+      <c r="A140" t="s">
+        <v>219</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>213</v>
@@ -4129,73 +4367,73 @@
         <v>187</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="68">
+    <row r="141" spans="1:4" ht="34">
       <c r="A141" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D141" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="34">
-      <c r="A142" t="s">
-        <v>219</v>
+        <v>221</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="323">
+      <c r="A142" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="34">
+        <v>224</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="323">
       <c r="A143" s="1" t="s">
-        <v>221</v>
+        <v>226</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" ht="323">
+      <c r="D143" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="409.6">
       <c r="A144" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>222</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="323">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="409.6">
       <c r="A145" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>222</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="409.6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="153">
       <c r="A146" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>228</v>
@@ -4204,12 +4442,12 @@
         <v>222</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="409.6">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="153">
       <c r="A147" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>228</v>
@@ -4218,12 +4456,12 @@
         <v>222</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="153">
       <c r="A148" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>228</v>
@@ -4237,7 +4475,7 @@
     </row>
     <row r="149" spans="1:4" ht="153">
       <c r="A149" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>228</v>
@@ -4249,118 +4487,112 @@
         <v>232</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="153">
+    <row r="150" spans="1:4" ht="85">
       <c r="A150" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="153">
+        <v>116</v>
+      </c>
+      <c r="B150" s="1"/>
+      <c r="C150" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="187">
       <c r="A151" s="1" t="s">
-        <v>235</v>
+        <v>118</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>222</v>
+        <v>119</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="85">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="34">
       <c r="A152" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B152" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="C152" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="187">
+    <row r="153" spans="1:4" ht="85">
       <c r="A153" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D153" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="34">
+    </row>
+    <row r="154" spans="1:4" ht="85">
       <c r="A154" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="85">
+    <row r="155" spans="1:4" ht="119">
       <c r="A155" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="85">
+    <row r="156" spans="1:4" ht="221">
       <c r="A156" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="119">
+    <row r="157" spans="1:4" ht="85">
       <c r="A157" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="221">
+    <row r="158" spans="1:4" ht="51">
       <c r="A158" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="85">
+    <row r="159" spans="1:4" ht="187">
       <c r="A159" s="1" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>133</v>
+        <v>237</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>117</v>
@@ -4368,142 +4600,142 @@
     </row>
     <row r="160" spans="1:4" ht="51">
       <c r="A160" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="187">
+    <row r="161" spans="1:4" ht="102">
       <c r="A161" s="1" t="s">
-        <v>236</v>
+        <v>140</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>237</v>
+        <v>141</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="51">
+    <row r="162" spans="1:4" ht="136">
       <c r="A162" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>47</v>
+        <v>143</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="102">
+    <row r="163" spans="1:4" ht="272">
       <c r="A163" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="136">
+    <row r="164" spans="1:4" ht="102">
       <c r="A164" s="1" t="s">
-        <v>142</v>
+        <v>238</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>143</v>
+        <v>47</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="272">
+    <row r="165" spans="1:4" ht="170">
       <c r="A165" s="1" t="s">
-        <v>144</v>
+        <v>239</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="102">
+    <row r="166" spans="1:4" ht="51">
       <c r="A166" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>117</v>
+        <v>243</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="170">
       <c r="A167" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="51">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="85">
       <c r="A168" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>242</v>
+        <v>80</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="170">
+    <row r="169" spans="1:4" ht="85">
       <c r="A169" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="85">
+    <row r="170" spans="1:4" ht="68">
       <c r="A170" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="85">
+    <row r="171" spans="1:4" ht="102">
       <c r="A171" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="68">
+    <row r="172" spans="1:4" ht="85">
       <c r="A172" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>73</v>
+        <v>253</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>243</v>
@@ -4511,10 +4743,10 @@
     </row>
     <row r="173" spans="1:4" ht="102">
       <c r="A173" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>251</v>
+        <v>62</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>243</v>
@@ -4522,98 +4754,104 @@
     </row>
     <row r="174" spans="1:4" ht="85">
       <c r="A174" s="1" t="s">
-        <v>252</v>
+        <v>148</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>253</v>
+        <v>149</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" ht="102">
+        <v>150</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="68">
       <c r="A175" s="1" t="s">
-        <v>254</v>
+        <v>152</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="85">
+        <v>150</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="68">
       <c r="A176" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="68">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="170">
       <c r="A177" s="1" t="s">
-        <v>152</v>
+        <v>255</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="68">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="85">
       <c r="A178" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>155</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="B178" s="3"/>
       <c r="C178" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="170">
-      <c r="A179" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>159</v>
+        <v>257</v>
+      </c>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" ht="85">
+      <c r="A179" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>74</v>
+        <v>257</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="85">
-      <c r="A180" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B180" s="3"/>
+      <c r="A180" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="C180" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D180" s="3"/>
+      <c r="D180" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="181" spans="1:4" ht="85">
       <c r="A181" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>257</v>
@@ -4624,10 +4862,10 @@
     </row>
     <row r="182" spans="1:4" ht="85">
       <c r="A182" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>257</v>
@@ -4637,8 +4875,8 @@
       </c>
     </row>
     <row r="183" spans="1:4" ht="85">
-      <c r="A183" s="3" t="s">
-        <v>262</v>
+      <c r="A183" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>263</v>
@@ -4646,30 +4884,26 @@
       <c r="C183" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D183" s="3" t="s">
+      <c r="D183" s="1" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="85">
-      <c r="A184" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>265</v>
-      </c>
+      <c r="A184" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B184" s="1"/>
       <c r="C184" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D184" s="3" t="s">
-        <v>260</v>
-      </c>
+      <c r="D184" s="1"/>
     </row>
     <row r="185" spans="1:4" ht="85">
-      <c r="A185" s="1" t="s">
-        <v>266</v>
+      <c r="A185" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>257</v>
@@ -4679,21 +4913,25 @@
       </c>
     </row>
     <row r="186" spans="1:4" ht="85">
-      <c r="A186" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B186" s="1"/>
+      <c r="A186" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="C186" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D186" s="1"/>
+      <c r="D186" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="187" spans="1:4" ht="85">
-      <c r="A187" s="3" t="s">
-        <v>258</v>
+      <c r="A187" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>257</v>
@@ -4703,11 +4941,11 @@
       </c>
     </row>
     <row r="188" spans="1:4" ht="85">
-      <c r="A188" s="3" t="s">
-        <v>261</v>
+      <c r="A188" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>257</v>
@@ -4718,7 +4956,7 @@
     </row>
     <row r="189" spans="1:4" ht="85">
       <c r="A189" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>263</v>
@@ -4732,10 +4970,10 @@
     </row>
     <row r="190" spans="1:4" ht="85">
       <c r="A190" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>257</v>
@@ -4746,35 +4984,35 @@
     </row>
     <row r="191" spans="1:4" ht="85">
       <c r="A191" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>263</v>
+        <v>271</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>257</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="85">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="68">
       <c r="A192" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>263</v>
+        <v>274</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>257</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" ht="85">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="51">
       <c r="A193" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>272</v>
@@ -4783,12 +5021,12 @@
         <v>257</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" ht="68">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="51">
       <c r="A194" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>272</v>
@@ -4797,12 +5035,12 @@
         <v>257</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="51">
       <c r="A195" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>272</v>
@@ -4816,7 +5054,7 @@
     </row>
     <row r="196" spans="1:4" ht="51">
       <c r="A196" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>272</v>
@@ -4828,12 +5066,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="51">
+    <row r="197" spans="1:4" ht="102">
       <c r="A197" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>257</v>
@@ -4842,12 +5080,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="51">
+    <row r="198" spans="1:4" ht="85">
       <c r="A198" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>257</v>
@@ -4856,9 +5094,9 @@
         <v>276</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="102">
+    <row r="199" spans="1:4" ht="85">
       <c r="A199" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>281</v>
@@ -4872,7 +5110,7 @@
     </row>
     <row r="200" spans="1:4" ht="85">
       <c r="A200" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>281</v>
@@ -4886,7 +5124,7 @@
     </row>
     <row r="201" spans="1:4" ht="85">
       <c r="A201" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>281</v>
@@ -4900,7 +5138,7 @@
     </row>
     <row r="202" spans="1:4" ht="85">
       <c r="A202" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>281</v>
@@ -4912,39 +5150,39 @@
         <v>276</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="85">
+    <row r="203" spans="1:4" ht="102">
       <c r="A203" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>281</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="B203" s="1"/>
       <c r="C203" s="2" t="s">
-        <v>257</v>
+        <v>161</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" ht="85">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="136">
       <c r="A204" s="1" t="s">
-        <v>286</v>
+        <v>166</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>281</v>
+        <v>164</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>257</v>
+        <v>161</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" ht="102">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="85">
       <c r="A205" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B205" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="C205" s="2" t="s">
         <v>161</v>
       </c>
@@ -4952,138 +5190,138 @@
         <v>162</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="136">
+    <row r="206" spans="1:4" ht="51">
       <c r="A206" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D206" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" ht="85">
+      <c r="D206" s="1"/>
+    </row>
+    <row r="207" spans="1:4" ht="51">
       <c r="A207" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D207" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" ht="51">
+      <c r="D207" s="1"/>
+    </row>
+    <row r="208" spans="1:4" ht="102">
       <c r="A208" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="B208" s="1"/>
       <c r="C208" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D208" s="1"/>
-    </row>
-    <row r="209" spans="1:4" ht="51">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="102">
       <c r="A209" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>171</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="B209" s="1"/>
       <c r="C209" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D209" s="1"/>
-    </row>
-    <row r="210" spans="1:4" ht="102">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="85">
       <c r="A210" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B210" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="C210" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" ht="102">
+      <c r="D210" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="85">
       <c r="A211" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B211" s="1"/>
+        <v>176</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="C211" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="D211" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="212" spans="1:4" ht="85">
       <c r="A212" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D212" s="1" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="213" spans="1:4" ht="85">
       <c r="A213" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D213" s="1" t="s">
+    </row>
+    <row r="214" spans="1:4" ht="102">
+      <c r="A214" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B214" s="1"/>
+      <c r="C214" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="51">
+      <c r="A215" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D215" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="85">
-      <c r="A214" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" ht="85">
-      <c r="A215" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" ht="102">
+    <row r="216" spans="1:4" ht="34">
       <c r="A216" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B216" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="C216" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="D216" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="217" spans="1:4" ht="51">
       <c r="A217" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>178</v>
@@ -5095,9 +5333,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="34">
+    <row r="218" spans="1:4" ht="51">
       <c r="A218" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>178</v>
@@ -5109,9 +5347,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="51">
+    <row r="219" spans="1:4" ht="68">
       <c r="A219" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>178</v>
@@ -5123,12 +5361,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="51">
+    <row r="220" spans="1:4" ht="68">
       <c r="A220" s="1" t="s">
-        <v>182</v>
+        <v>287</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>178</v>
+        <v>80</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>178</v>
@@ -5137,54 +5375,54 @@
         <v>74</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="68">
-      <c r="A221" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>178</v>
+    <row r="221" spans="1:4" ht="102">
+      <c r="A221" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" ht="68">
-      <c r="A222" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>80</v>
+        <v>343</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="221">
+      <c r="A222" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" ht="102">
+        <v>343</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="68">
       <c r="A223" s="4" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D223" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" ht="221">
+      <c r="D223" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="136">
       <c r="A224" s="4" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>343</v>
@@ -5193,9 +5431,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="68">
+    <row r="225" spans="1:4" ht="51">
       <c r="A225" s="4" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B225" s="4" t="s">
         <v>293</v>
@@ -5207,12 +5445,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="136">
+    <row r="226" spans="1:4" ht="51">
       <c r="A226" s="4" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>343</v>
@@ -5221,26 +5459,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="51">
+    <row r="227" spans="1:4" ht="85">
       <c r="A227" s="4" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D227" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" ht="51">
+      <c r="D227" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="221">
       <c r="A228" s="4" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>343</v>
@@ -5249,26 +5487,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="85">
+    <row r="229" spans="1:4" ht="68">
       <c r="A229" s="4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D229" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" ht="221">
+      <c r="D229" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="136">
       <c r="A230" s="4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>343</v>
@@ -5277,9 +5515,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="68">
+    <row r="231" spans="1:4" ht="51">
       <c r="A231" s="4" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B231" s="4" t="s">
         <v>293</v>
@@ -5291,12 +5529,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="136">
+    <row r="232" spans="1:4" ht="51">
       <c r="A232" s="4" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>343</v>
@@ -5305,26 +5543,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="51">
+    <row r="233" spans="1:4" ht="102">
       <c r="A233" s="4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D233" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" ht="51">
+      <c r="D233" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="221">
       <c r="A234" s="4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>343</v>
@@ -5333,26 +5571,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="102">
+    <row r="235" spans="1:4" ht="51">
       <c r="A235" s="4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D235" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" ht="221">
+      <c r="D235" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="136">
       <c r="A236" s="4" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>343</v>
@@ -5363,7 +5601,7 @@
     </row>
     <row r="237" spans="1:4" ht="51">
       <c r="A237" s="4" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B237" s="4" t="s">
         <v>293</v>
@@ -5375,12 +5613,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="136">
+    <row r="238" spans="1:4" ht="51">
       <c r="A238" s="4" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>343</v>
@@ -5389,12 +5627,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="51">
+    <row r="239" spans="1:4" ht="85">
       <c r="A239" s="4" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>343</v>
@@ -5403,26 +5641,26 @@
         <v>187</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="51">
+    <row r="240" spans="1:4" ht="136">
       <c r="A240" s="4" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D240" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" ht="85">
+      <c r="D240" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" ht="119">
       <c r="A241" s="4" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>343</v>
@@ -5431,12 +5669,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="136">
+    <row r="242" spans="1:4" ht="356">
       <c r="A242" s="4" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>343</v>
@@ -5445,12 +5683,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="119">
+    <row r="243" spans="1:4" ht="68">
       <c r="A243" s="4" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>343</v>
@@ -5459,37 +5697,37 @@
         <v>187</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="356">
-      <c r="A244" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="B244" s="4" t="s">
-        <v>318</v>
+    <row r="244" spans="1:4" ht="409.6">
+      <c r="A244" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D244" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" ht="68">
-      <c r="A245" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="B245" s="4" t="s">
-        <v>320</v>
+        <v>333</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="409.6">
+      <c r="A245" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D245" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" ht="409.6">
+        <v>333</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" ht="306">
       <c r="A246" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>323</v>
@@ -5497,79 +5735,73 @@
       <c r="C246" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D246" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" ht="409.6">
-      <c r="A247" s="3" t="s">
-        <v>325</v>
+      <c r="D246" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" ht="272">
+      <c r="A247" s="4" t="s">
+        <v>328</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D247" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" ht="306">
-      <c r="A248" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B248" s="3" t="s">
-        <v>323</v>
+      <c r="D247" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" ht="221">
+      <c r="A248" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>331</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>333</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" ht="272">
-      <c r="A249" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="B249" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D249" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" ht="221">
-      <c r="A250" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B250" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D250" s="4" t="s">
         <v>332</v>
       </c>
     </row>
+    <row r="249" spans="1:4" ht="85">
+      <c r="A249" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B249" s="3"/>
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" spans="1:4" ht="85">
+      <c r="A250" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
     <row r="251" spans="1:4" ht="85">
-      <c r="A251" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B251" s="3"/>
-      <c r="D251" s="3"/>
+      <c r="A251" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="252" spans="1:4" ht="85">
       <c r="A252" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>260</v>
@@ -5577,64 +5809,70 @@
     </row>
     <row r="253" spans="1:4" ht="85">
       <c r="A253" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D253" s="3" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="85">
-      <c r="A254" s="3" t="s">
-        <v>262</v>
+      <c r="A254" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="D254" s="3" t="s">
+      <c r="D254" s="1" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="85">
-      <c r="A255" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D255" s="3" t="s">
-        <v>260</v>
-      </c>
+      <c r="A255" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D255" s="1"/>
     </row>
     <row r="256" spans="1:4" ht="85">
-      <c r="A256" s="1" t="s">
-        <v>266</v>
+      <c r="A256" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="85">
-      <c r="A257" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B257" s="1"/>
+      <c r="A257" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="C257" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="D257" s="1"/>
+      <c r="D257" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="258" spans="1:4" ht="85">
-      <c r="A258" s="3" t="s">
-        <v>258</v>
+      <c r="A258" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>335</v>
@@ -5644,11 +5882,11 @@
       </c>
     </row>
     <row r="259" spans="1:4" ht="85">
-      <c r="A259" s="3" t="s">
-        <v>261</v>
+      <c r="A259" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>335</v>
@@ -5659,7 +5897,7 @@
     </row>
     <row r="260" spans="1:4" ht="85">
       <c r="A260" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>263</v>
@@ -5673,10 +5911,10 @@
     </row>
     <row r="261" spans="1:4" ht="85">
       <c r="A261" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>335</v>
@@ -5687,35 +5925,35 @@
     </row>
     <row r="262" spans="1:4" ht="85">
       <c r="A262" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>263</v>
+        <v>271</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>335</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" ht="85">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" ht="68">
       <c r="A263" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>263</v>
+        <v>274</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>335</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" ht="85">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" ht="51">
       <c r="A264" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>272</v>
@@ -5724,12 +5962,12 @@
         <v>335</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" ht="68">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" ht="51">
       <c r="A265" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>272</v>
@@ -5738,12 +5976,12 @@
         <v>335</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="51">
       <c r="A266" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>272</v>
@@ -5757,7 +5995,7 @@
     </row>
     <row r="267" spans="1:4" ht="51">
       <c r="A267" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>272</v>
@@ -5769,12 +6007,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="51">
+    <row r="268" spans="1:4" ht="102">
       <c r="A268" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>335</v>
@@ -5783,12 +6021,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="51">
+    <row r="269" spans="1:4" ht="85">
       <c r="A269" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>335</v>
@@ -5797,9 +6035,9 @@
         <v>276</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="102">
+    <row r="270" spans="1:4" ht="85">
       <c r="A270" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>281</v>
@@ -5813,7 +6051,7 @@
     </row>
     <row r="271" spans="1:4" ht="85">
       <c r="A271" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>281</v>
@@ -5827,7 +6065,7 @@
     </row>
     <row r="272" spans="1:4" ht="85">
       <c r="A272" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>281</v>
@@ -5841,7 +6079,7 @@
     </row>
     <row r="273" spans="1:4" ht="85">
       <c r="A273" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>281</v>
@@ -5853,37 +6091,37 @@
         <v>276</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="85">
-      <c r="A274" s="1" t="s">
-        <v>285</v>
+    <row r="274" spans="1:4" ht="51">
+      <c r="A274" s="7" t="s">
+        <v>336</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>281</v>
+        <v>339</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" ht="85">
-      <c r="A275" s="1" t="s">
-        <v>286</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" ht="34">
+      <c r="A275" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>281</v>
+        <v>339</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" ht="51">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="34">
       <c r="A276" s="7" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>339</v>
@@ -5895,9 +6133,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="34">
+    <row r="277" spans="1:4" ht="51">
       <c r="A277" s="7" t="s">
-        <v>337</v>
+        <v>4</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>339</v>
@@ -5909,9 +6147,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="34">
+    <row r="278" spans="1:4" ht="68">
       <c r="A278" s="7" t="s">
-        <v>338</v>
+        <v>5</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>339</v>
@@ -5923,9 +6161,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="51">
+    <row r="279" spans="1:4" ht="68">
       <c r="A279" s="7" t="s">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>339</v>
@@ -5937,71 +6175,71 @@
         <v>74</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="68">
-      <c r="A280" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B280" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D280" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="281" spans="1:4" ht="68">
-      <c r="A281" s="7" t="s">
-        <v>184</v>
+    <row r="280" spans="1:4" ht="34">
+      <c r="A280" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C280" s="3"/>
+    </row>
+    <row r="281" spans="1:4" ht="323">
+      <c r="A281" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>339</v>
+        <v>224</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="282" spans="1:4" ht="34">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" ht="323">
       <c r="A282" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C282" s="3"/>
-    </row>
-    <row r="283" spans="1:4" ht="323">
+        <v>226</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" ht="409.6">
       <c r="A283" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>342</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="284" spans="1:4" ht="323">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" ht="409.6">
       <c r="A284" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>342</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" ht="409.6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" ht="153">
       <c r="A285" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>228</v>
@@ -6010,12 +6248,12 @@
         <v>342</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" ht="409.6">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" ht="153">
       <c r="A286" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>228</v>
@@ -6024,12 +6262,12 @@
         <v>342</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="153">
       <c r="A287" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>228</v>
@@ -6043,7 +6281,7 @@
     </row>
     <row r="288" spans="1:4" ht="153">
       <c r="A288" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>228</v>
@@ -6055,39 +6293,39 @@
         <v>232</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="153">
+    <row r="289" spans="1:4" ht="68">
       <c r="A289" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B289" s="1" t="s">
-        <v>228</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B289" s="1"/>
       <c r="C289" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D289" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4" ht="153">
+        <v>321</v>
+      </c>
+      <c r="D289" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" ht="51">
       <c r="A290" s="1" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>228</v>
+        <v>80</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4" ht="68">
+        <v>321</v>
+      </c>
+      <c r="D290" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" ht="204">
       <c r="A291" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B291" s="1"/>
+        <v>197</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C291" s="1" t="s">
         <v>321</v>
       </c>
@@ -6095,12 +6333,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="51">
+    <row r="292" spans="1:4" ht="204">
       <c r="A292" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>321</v>
@@ -6109,12 +6347,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="204">
+    <row r="293" spans="1:4" ht="68">
       <c r="A293" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>321</v>
@@ -6123,12 +6361,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="204">
+    <row r="294" spans="1:4" ht="68">
       <c r="A294" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>321</v>
@@ -6137,26 +6375,21 @@
         <v>74</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="68">
+    <row r="295" spans="1:4" ht="51">
       <c r="A295" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B295" s="1" t="s">
-        <v>202</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B295" s="1"/>
       <c r="C295" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D295" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="296" spans="1:4" ht="68">
+    </row>
+    <row r="296" spans="1:4" ht="255">
       <c r="A296" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>321</v>
@@ -6165,91 +6398,96 @@
         <v>74</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="51">
+    <row r="297" spans="1:4" ht="204">
       <c r="A297" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B297" s="1"/>
+        <v>208</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="C297" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" ht="255">
+      <c r="D297" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" ht="409.6">
       <c r="A298" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B298" s="1" t="s">
-        <v>207</v>
+        <v>344</v>
+      </c>
+      <c r="B298" s="3" t="s">
+        <v>345</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D298" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="299" spans="1:4" ht="204">
+        <v>348</v>
+      </c>
+      <c r="D298" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" ht="409.6">
       <c r="A299" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B299" s="1" t="s">
-        <v>200</v>
+        <v>347</v>
+      </c>
+      <c r="B299" s="3" t="s">
+        <v>345</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D299" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="300" spans="1:4" ht="409.6">
-      <c r="A300" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B300" s="3" t="s">
-        <v>345</v>
+        <v>348</v>
+      </c>
+      <c r="D299" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" ht="306">
+      <c r="A300" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B300" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>348</v>
       </c>
       <c r="D300" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4" ht="409.6">
-      <c r="A301" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B301" s="3" t="s">
-        <v>345</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" ht="306">
+      <c r="A301" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B301" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D301" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="302" spans="1:4" ht="306">
-      <c r="A302" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B302" s="4" t="s">
-        <v>212</v>
+      <c r="D301" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" ht="34">
+      <c r="A302" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D302" s="3" t="s">
+      <c r="D302" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="306">
-      <c r="A303" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B303" s="4" t="s">
-        <v>212</v>
+    <row r="303" spans="1:4" ht="68">
+      <c r="A303" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>348</v>
@@ -6259,11 +6497,11 @@
       </c>
     </row>
     <row r="304" spans="1:4" ht="34">
-      <c r="A304" s="1" t="s">
-        <v>215</v>
+      <c r="A304" t="s">
+        <v>219</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>348</v>
@@ -6272,84 +6510,330 @@
         <v>187</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="68">
+    <row r="305" spans="1:4" ht="51">
       <c r="A305" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C305" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D305" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4" ht="34">
-      <c r="A306" t="s">
-        <v>219</v>
+        <v>242</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D305" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" ht="136">
+      <c r="A306" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D306" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="307" spans="1:4" ht="51">
+        <v>350</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D306" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" ht="238">
       <c r="A307" s="1" t="s">
-        <v>241</v>
+        <v>351</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C307" s="3" t="s">
-        <v>243</v>
+        <v>352</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D307" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="308" spans="1:4">
-      <c r="A308" s="1"/>
-      <c r="B308" s="1"/>
-      <c r="D308" s="3"/>
-    </row>
-    <row r="309" spans="1:4">
-      <c r="A309" s="1"/>
-      <c r="B309" s="1"/>
-      <c r="D309" s="3"/>
-    </row>
-    <row r="310" spans="1:4">
-      <c r="A310" s="1"/>
-      <c r="B310" s="1"/>
-      <c r="D310" s="3"/>
-    </row>
-    <row r="311" spans="1:4">
-      <c r="A311" s="1"/>
-      <c r="B311" s="1"/>
-      <c r="D311" s="3"/>
-    </row>
-    <row r="312" spans="1:4">
-      <c r="A312" s="1"/>
-      <c r="B312" s="1"/>
-      <c r="D312" s="1"/>
-    </row>
-    <row r="313" spans="1:4">
-      <c r="A313" s="1"/>
-      <c r="B313" s="1"/>
-      <c r="D313" s="1"/>
-    </row>
-    <row r="314" spans="1:4">
-      <c r="A314" s="1"/>
-      <c r="B314" s="1"/>
-      <c r="D314" s="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" ht="289">
+      <c r="A308" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D308" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" ht="85">
+      <c r="A309" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D309" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" ht="51">
+      <c r="A310" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" ht="306">
+      <c r="A311" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" ht="51">
+      <c r="A312" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" ht="306">
+      <c r="A313" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" ht="238">
+      <c r="A314" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" ht="170">
+      <c r="A315" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" ht="68">
+      <c r="A316" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" ht="102">
+      <c r="A317" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" ht="102">
+      <c r="A318" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" ht="238">
+      <c r="A319" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" ht="238">
+      <c r="A320" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" ht="51">
+      <c r="A321" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" ht="85">
+      <c r="A322" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" ht="221">
+      <c r="A323" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" ht="187">
+      <c r="A324" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" ht="119">
+      <c r="A325" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" ht="34">
+      <c r="A326" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" ht="34">
+      <c r="A327" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D327" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D316" xr:uid="{B2262C64-3841-164B-B8C6-01B4F63C9295}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>